<commit_message>
cigna global code changes
</commit_message>
<xml_diff>
--- a/Input/cigna/benefits.xlsx
+++ b/Input/cigna/benefits.xlsx
@@ -292,10 +292,10 @@
     <t xml:space="preserve">Annually</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-10-15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024-04-15</t>
+    <t xml:space="preserve">2024-09-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-02-15</t>
   </si>
   <si>
     <t xml:space="preserve">Cigna</t>
@@ -393,6 +393,11 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -400,14 +405,10 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -452,7 +453,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -465,16 +466,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -487,12 +484,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -558,43 +555,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:BG5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AW1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BG4" activeCellId="0" sqref="BG4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AX1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BC3" activeCellId="0" sqref="BC3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="81.7"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="42.1"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="33.76"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="10" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="145.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="63.21"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="19" min="16" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="30.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="45.84"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="40" min="22" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="47.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="62.24"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="48" min="43" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="27.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="19.72"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="55" min="51" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="0" width="21.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="58" min="57" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="0" width="38.9"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="60" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1082,7 +1070,7 @@
       <c r="BA3" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="BG3" s="6" t="s">
+      <c r="BG3" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1222,12 +1210,12 @@
       <c r="AX4" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="BG4" s="7" t="s">
+      <c r="BG4" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="BG5" s="7" t="s">
+      <c r="BG5" s="6" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cigna healthguard rates update
</commit_message>
<xml_diff>
--- a/Input/cigna/benefits.xlsx
+++ b/Input/cigna/benefits.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="113">
   <si>
     <t xml:space="preserve">PlanName</t>
   </si>
@@ -196,9 +196,6 @@
     <t xml:space="preserve">addons</t>
   </si>
   <si>
-    <t xml:space="preserve">conversionRate</t>
-  </si>
-  <si>
     <t xml:space="preserve">International Plus</t>
   </si>
   <si>
@@ -295,10 +292,10 @@
     <t xml:space="preserve">Annually</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-10-15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024-04-15</t>
+    <t xml:space="preserve">2024-09-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-02-15</t>
   </si>
   <si>
     <t xml:space="preserve">Cigna</t>
@@ -325,7 +322,7 @@
     <t xml:space="preserve">Covered in full up to 30 sessions</t>
   </si>
   <si>
-    <t xml:space="preserve">Preventative dental treatment covered up to USD 300 (Enhanced option available)</t>
+    <t xml:space="preserve">Preventative dental treatment covered up to USD 3,000 (Enhanced option available)</t>
   </si>
   <si>
     <t xml:space="preserve">Enhanced Wellness availalable with health connect module</t>
@@ -355,8 +352,7 @@
     <t xml:space="preserve">Covered in full up to 15 sessions</t>
   </si>
   <si>
-    <t xml:space="preserve">Preventative dental treatment covered up to USD 150
-(Enhanced option available)</t>
+    <t xml:space="preserve">Preventative dental treatment covered up to AED 550 (Enhanced option available)</t>
   </si>
   <si>
     <t xml:space="preserve">Homeopathy, Ayurveda and Chinese medicine covered up to USD 1,000</t>
@@ -374,7 +370,7 @@
     <numFmt numFmtId="165" formatCode="0.00%"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -397,14 +393,19 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
@@ -452,13 +453,9 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -469,7 +466,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -477,12 +474,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -494,6 +491,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF222222"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -502,13 +559,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BH5"/>
+  <dimension ref="A1:BG5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BF1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BI7" activeCellId="0" sqref="BI7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AX1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BC3" activeCellId="0" sqref="BC3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.06"/>
@@ -520,15 +577,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="63.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="30.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="45.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="18.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="47.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="62.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="27.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="19.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="0" width="21.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="0" width="40.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="0" width="25.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="0" width="38.9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -703,471 +757,465 @@
       <c r="BF1" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BG1" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="BH1" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>63</v>
-      </c>
       <c r="F2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="I2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="N2" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="N2" s="0" t="s">
+      <c r="O2" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="P2" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q2" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="R2" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="S2" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="Q2" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="R2" s="0" t="s">
+      <c r="T2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="U2" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="S2" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="T2" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="U2" s="0" t="s">
+      <c r="V2" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="V2" s="0" t="s">
+      <c r="W2" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="W2" s="0" t="s">
+      <c r="X2" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="X2" s="0" t="s">
+      <c r="Z2" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="Z2" s="0" t="s">
+      <c r="AA2" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="AA2" s="0" t="s">
+      <c r="AB2" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="AB2" s="0" t="s">
+      <c r="AC2" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="AC2" s="0" t="s">
+      <c r="AD2" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="AD2" s="0" t="s">
+      <c r="AE2" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="AE2" s="0" t="s">
+      <c r="AF2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG2" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="AF2" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG2" s="0" t="s">
+      <c r="AH2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI2" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ2" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="AH2" s="0" t="s">
+      <c r="AK2" s="1" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="AL2" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="AI2" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="AJ2" s="0" t="s">
+      <c r="AO2" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="AK2" s="2" t="n">
-        <v>0.055</v>
-      </c>
-      <c r="AL2" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO2" s="0" t="s">
+      <c r="AP2" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="AP2" s="0" t="s">
+      <c r="AQ2" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="AQ2" s="0" t="s">
-        <v>85</v>
-      </c>
       <c r="AR2" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AS2" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AT2" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AU2" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AV2" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AW2" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="AS2" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AT2" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AU2" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AV2" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AW2" s="3" t="s">
+      <c r="AX2" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="AX2" s="0" t="s">
+      <c r="AY2" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="AY2" s="0" t="s">
+      <c r="BA2" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="BA2" s="0" t="s">
+      <c r="BB2" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="BB2" s="4" t="s">
+      <c r="BC2" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="BC2" s="4" t="s">
+      <c r="BD2" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="BD2" s="0" t="s">
+      <c r="BE2" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="BE2" s="0" t="s">
+      <c r="BF2" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="BF2" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="BG2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="BH2" s="0" t="n">
-        <v>3.675</v>
+      <c r="BG2" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="4" t="n">
+        <v>2000000</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="N3" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="5" t="n">
-        <v>2000000</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="Q3" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="U3" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="V3" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="X3" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z3" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA3" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB3" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC3" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD3" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE3" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF3" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG3" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH3" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI3" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ3" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK3" s="1" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="AL3" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AO3" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP3" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="AQ3" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR3" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AS3" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AT3" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AU3" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AV3" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AW3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AX3" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="AZ3" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="BA3" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="BG3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="4" t="n">
+        <v>750000</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" s="0" t="s">
+      <c r="F4" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="H4" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q3" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="R3" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="S3" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="T3" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="U3" s="0" t="s">
+      <c r="I4" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="T4" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="U4" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="V4" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="V3" s="0" t="s">
+      <c r="W4" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="W3" s="0" t="s">
+      <c r="X4" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="X3" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z3" s="0" t="s">
+      <c r="Z4" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA4" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB4" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC4" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="AA3" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="AB3" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC3" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="AD3" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="AE3" s="0" t="s">
+      <c r="AD4" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="AE4" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF4" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG4" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="AF3" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG3" s="0" t="s">
+      <c r="AH4" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI4" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ4" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="AH3" s="0" t="s">
+      <c r="AK4" s="1" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="AL4" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="AI3" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="AJ3" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="AK3" s="2" t="n">
-        <v>0.055</v>
-      </c>
-      <c r="AL3" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO3" s="0" t="s">
+      <c r="AO4" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="AP4" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="AP3" s="0" t="s">
+      <c r="AQ4" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="AQ3" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="AR3" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AS3" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AT3" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AU3" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AV3" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AW3" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AX3" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="AZ3" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="BA3" s="6" t="s">
+      <c r="AR4" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AS4" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AT4" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AU4" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AV4" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="AW4" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="BG3" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="B4" s="5" t="n">
-        <v>750000</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="M4" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="N4" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q4" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="R4" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="S4" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="T4" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="U4" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="V4" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="W4" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="X4" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z4" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA4" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="AB4" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC4" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="AD4" s="0" t="s">
+      <c r="AX4" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="AE4" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF4" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG4" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH4" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="AI4" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="AJ4" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="AK4" s="2" t="n">
-        <v>0.055</v>
-      </c>
-      <c r="AL4" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO4" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="AP4" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="AQ4" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="AR4" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AS4" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AT4" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AU4" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AV4" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AW4" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="AX4" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="BG4" s="3" t="s">
+      <c r="BG4" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="BG5" s="3" t="s">
+      <c r="BG5" s="6" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>